<commit_message>
Add Veljko Milutinovic to primary dataset authors list
</commit_message>
<xml_diff>
--- a/data/UB_cs_authors.xlsx
+++ b/data/UB_cs_authors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Markov folder\__nastava\asm\Projekat\2019-2020\PZ2\Podaci\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\ASM\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0026FD29-3D05-4453-A67D-27D79A992682}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAEA367A-A351-4F8F-802C-A86493F861DF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2190" yWindow="2010" windowWidth="24465" windowHeight="11340" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="matematicki fakultet" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="227">
   <si>
     <t>Ime</t>
   </si>
@@ -697,6 +697,12 @@
   </si>
   <si>
     <t>O</t>
+  </si>
+  <si>
+    <t>Veljko</t>
+  </si>
+  <si>
+    <t>Milutinovic</t>
   </si>
 </sst>
 </file>
@@ -1070,7 +1076,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2:C40"/>
     </sheetView>
   </sheetViews>
@@ -1730,10 +1736,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E40"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2387,6 +2393,20 @@
         <v>77</v>
       </c>
       <c r="E40" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>225</v>
+      </c>
+      <c r="B41" t="s">
+        <v>226</v>
+      </c>
+      <c r="D41" t="s">
+        <v>77</v>
+      </c>
+      <c r="E41" t="s">
         <v>78</v>
       </c>
     </row>

</xml_diff>